<commit_message>
bovis defining SNPs and filter region update
</commit_message>
<xml_diff>
--- a/portable_scripts/script_dependents/Mycobacterium_bovis/Filtered_Regions.xlsx
+++ b/portable_scripts/script_dependents/Mycobacterium_bovis/Filtered_Regions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="56460" yWindow="4725" windowWidth="33045" windowHeight="23595" tabRatio="500"/>
+    <workbookView xWindow="56460" yWindow="4728" windowWidth="33048" windowHeight="23592" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="New groupings" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4071" uniqueCount="1043">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4088" uniqueCount="1047">
   <si>
     <t>Subgroup-1A</t>
   </si>
@@ -3153,6 +3153,18 @@
   </si>
   <si>
     <t>2607071</t>
+  </si>
+  <si>
+    <t>3720608</t>
+  </si>
+  <si>
+    <t>3773092</t>
+  </si>
+  <si>
+    <t>432342</t>
+  </si>
+  <si>
+    <t>3668907</t>
   </si>
 </sst>
 </file>
@@ -5905,74 +5917,74 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DS452"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CL1" workbookViewId="0">
-      <selection activeCell="CR48" sqref="CR48:CR75"/>
+    <sheetView tabSelected="1" topLeftCell="BK1" workbookViewId="0">
+      <selection activeCell="BP23" sqref="BP23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.125" style="1" customWidth="1"/>
-    <col min="6" max="7" width="10.875" style="1"/>
-    <col min="8" max="8" width="15.875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.875" style="1"/>
-    <col min="11" max="11" width="13.625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="15.375" style="1" customWidth="1"/>
-    <col min="13" max="14" width="10.875" style="1"/>
-    <col min="15" max="15" width="11.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.59765625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.59765625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.59765625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.09765625" style="1" customWidth="1"/>
+    <col min="6" max="7" width="10.8984375" style="1"/>
+    <col min="8" max="8" width="15.8984375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.3984375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.8984375" style="1"/>
+    <col min="11" max="11" width="13.59765625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="15.3984375" style="1" customWidth="1"/>
+    <col min="13" max="14" width="10.8984375" style="1"/>
+    <col min="15" max="15" width="11.59765625" style="1" customWidth="1"/>
     <col min="16" max="16" width="15" style="1" customWidth="1"/>
-    <col min="17" max="17" width="10.875" style="1"/>
+    <col min="17" max="17" width="10.8984375" style="1"/>
     <col min="18" max="18" width="13" style="1" customWidth="1"/>
-    <col min="19" max="19" width="10.875" style="1"/>
-    <col min="20" max="20" width="16.125" style="1" customWidth="1"/>
-    <col min="21" max="22" width="10.875" style="1"/>
-    <col min="23" max="23" width="15.375" style="8" customWidth="1"/>
-    <col min="24" max="24" width="15.625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="10.8984375" style="1"/>
+    <col min="20" max="20" width="16.09765625" style="1" customWidth="1"/>
+    <col min="21" max="22" width="10.8984375" style="1"/>
+    <col min="23" max="23" width="15.3984375" style="8" customWidth="1"/>
+    <col min="24" max="24" width="15.59765625" style="1" customWidth="1"/>
     <col min="25" max="25" width="13.5" style="8" customWidth="1"/>
-    <col min="26" max="27" width="11.875" style="1" customWidth="1"/>
-    <col min="28" max="36" width="10.875" style="1"/>
-    <col min="37" max="37" width="10.875" style="8"/>
-    <col min="38" max="52" width="10.875" style="1"/>
-    <col min="53" max="53" width="19.375" style="1" customWidth="1"/>
+    <col min="26" max="27" width="11.8984375" style="1" customWidth="1"/>
+    <col min="28" max="36" width="10.8984375" style="1"/>
+    <col min="37" max="37" width="10.8984375" style="8"/>
+    <col min="38" max="52" width="10.8984375" style="1"/>
+    <col min="53" max="53" width="19.3984375" style="1" customWidth="1"/>
     <col min="54" max="54" width="14" style="1" customWidth="1"/>
-    <col min="55" max="57" width="10.875" style="1"/>
-    <col min="58" max="58" width="15.625" style="1" customWidth="1"/>
-    <col min="59" max="59" width="10.875" style="1"/>
-    <col min="60" max="60" width="13.375" style="1" customWidth="1"/>
-    <col min="61" max="61" width="13.625" style="1" customWidth="1"/>
-    <col min="62" max="62" width="14.625" style="1" customWidth="1"/>
-    <col min="63" max="63" width="10.875" style="1"/>
-    <col min="64" max="64" width="15.375" style="1" customWidth="1"/>
-    <col min="65" max="69" width="12.875" style="1" customWidth="1"/>
-    <col min="70" max="70" width="10.875" style="1"/>
-    <col min="71" max="71" width="13.375" style="1" customWidth="1"/>
-    <col min="72" max="73" width="12.625" style="1" customWidth="1"/>
-    <col min="74" max="79" width="10.875" style="1"/>
-    <col min="80" max="83" width="12.875" style="1" customWidth="1"/>
-    <col min="84" max="85" width="15.375" style="1" customWidth="1"/>
-    <col min="86" max="94" width="10.875" style="1"/>
-    <col min="95" max="95" width="14.625" style="1" customWidth="1"/>
+    <col min="55" max="57" width="10.8984375" style="1"/>
+    <col min="58" max="58" width="15.59765625" style="1" customWidth="1"/>
+    <col min="59" max="59" width="10.8984375" style="1"/>
+    <col min="60" max="60" width="13.3984375" style="1" customWidth="1"/>
+    <col min="61" max="61" width="13.59765625" style="1" customWidth="1"/>
+    <col min="62" max="62" width="14.59765625" style="1" customWidth="1"/>
+    <col min="63" max="63" width="10.8984375" style="1"/>
+    <col min="64" max="64" width="15.3984375" style="1" customWidth="1"/>
+    <col min="65" max="69" width="12.8984375" style="1" customWidth="1"/>
+    <col min="70" max="70" width="10.8984375" style="1"/>
+    <col min="71" max="71" width="13.3984375" style="1" customWidth="1"/>
+    <col min="72" max="73" width="12.59765625" style="1" customWidth="1"/>
+    <col min="74" max="79" width="10.8984375" style="1"/>
+    <col min="80" max="83" width="12.8984375" style="1" customWidth="1"/>
+    <col min="84" max="85" width="15.3984375" style="1" customWidth="1"/>
+    <col min="86" max="94" width="10.8984375" style="1"/>
+    <col min="95" max="95" width="14.59765625" style="1" customWidth="1"/>
     <col min="96" max="96" width="16" style="1" customWidth="1"/>
-    <col min="97" max="97" width="10.875" style="1"/>
-    <col min="98" max="98" width="13.875" style="1" customWidth="1"/>
-    <col min="99" max="99" width="12.625" style="1" customWidth="1"/>
-    <col min="100" max="101" width="10.875" style="1"/>
-    <col min="102" max="102" width="12.125" style="1" customWidth="1"/>
-    <col min="103" max="103" width="10.875" style="1"/>
+    <col min="97" max="97" width="10.8984375" style="1"/>
+    <col min="98" max="98" width="13.8984375" style="1" customWidth="1"/>
+    <col min="99" max="99" width="12.59765625" style="1" customWidth="1"/>
+    <col min="100" max="101" width="10.8984375" style="1"/>
+    <col min="102" max="102" width="12.09765625" style="1" customWidth="1"/>
+    <col min="103" max="103" width="10.8984375" style="1"/>
     <col min="104" max="104" width="15" style="1" customWidth="1"/>
     <col min="105" max="110" width="13" style="1" customWidth="1"/>
-    <col min="111" max="114" width="10.875" style="1"/>
-    <col min="115" max="115" width="16.125" style="1" customWidth="1"/>
+    <col min="111" max="114" width="10.8984375" style="1"/>
+    <col min="115" max="115" width="16.09765625" style="1" customWidth="1"/>
     <col min="116" max="116" width="16" style="1" bestFit="1" customWidth="1"/>
     <col min="117" max="117" width="16" style="1" customWidth="1"/>
-    <col min="118" max="16384" width="10.875" style="1"/>
+    <col min="118" max="16384" width="10.8984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>228</v>
       </c>
@@ -6343,7 +6355,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="2" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>44</v>
       </c>
@@ -6714,7 +6726,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="3" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>45</v>
       </c>
@@ -7031,7 +7043,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="4" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>151</v>
       </c>
@@ -7348,7 +7360,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="5" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>152</v>
       </c>
@@ -7662,7 +7674,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="6" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>249</v>
       </c>
@@ -7974,7 +7986,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="7" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>153</v>
       </c>
@@ -8287,7 +8299,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="8" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>154</v>
       </c>
@@ -8591,7 +8603,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="9" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>155</v>
       </c>
@@ -8892,7 +8904,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="10" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>250</v>
       </c>
@@ -9193,7 +9205,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="11" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>156</v>
       </c>
@@ -9492,7 +9504,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="12" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>157</v>
       </c>
@@ -9786,7 +9798,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="13" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>158</v>
       </c>
@@ -10077,7 +10089,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="14" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>159</v>
       </c>
@@ -10356,7 +10368,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="15" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>160</v>
       </c>
@@ -10535,6 +10547,9 @@
       <c r="BM15" s="6" t="s">
         <v>795</v>
       </c>
+      <c r="BN15" s="1" t="s">
+        <v>810</v>
+      </c>
       <c r="BO15" s="6" t="s">
         <v>797</v>
       </c>
@@ -10632,7 +10647,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="16" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>161</v>
       </c>
@@ -10904,7 +10919,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="17" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>162</v>
       </c>
@@ -11081,6 +11096,9 @@
       </c>
       <c r="BO17" s="6" t="s">
         <v>778</v>
+      </c>
+      <c r="BP17" s="1" t="s">
+        <v>810</v>
       </c>
       <c r="BQ17" s="6" t="s">
         <v>796</v>
@@ -11172,7 +11190,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="18" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>163</v>
       </c>
@@ -11434,7 +11452,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="19" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>164</v>
       </c>
@@ -11599,6 +11617,9 @@
       </c>
       <c r="BM19" s="6" t="s">
         <v>778</v>
+      </c>
+      <c r="BO19" s="1" t="s">
+        <v>810</v>
       </c>
       <c r="BQ19" s="6" t="s">
         <v>814</v>
@@ -11684,7 +11705,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="20" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>251</v>
       </c>
@@ -11932,7 +11953,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="21" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>46</v>
       </c>
@@ -12099,7 +12120,9 @@
       <c r="BM21" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="BQ21" s="6"/>
+      <c r="BQ21" s="6" t="s">
+        <v>810</v>
+      </c>
       <c r="BR21" s="1" t="s">
         <v>367</v>
       </c>
@@ -12178,7 +12201,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="22" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>47</v>
       </c>
@@ -12342,6 +12365,9 @@
       <c r="BL22" s="6" t="s">
         <v>795</v>
       </c>
+      <c r="BM22" s="1" t="s">
+        <v>810</v>
+      </c>
       <c r="BR22" s="1" t="s">
         <v>352</v>
       </c>
@@ -12400,7 +12426,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="23" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>252</v>
       </c>
@@ -12622,7 +12648,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="24" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>48</v>
       </c>
@@ -12844,7 +12870,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="25" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>49</v>
       </c>
@@ -13045,7 +13071,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="26" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>50</v>
       </c>
@@ -13228,7 +13254,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="27" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>51</v>
       </c>
@@ -13408,7 +13434,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="28" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>165</v>
       </c>
@@ -13585,7 +13611,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="29" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>166</v>
       </c>
@@ -13707,6 +13733,9 @@
       <c r="BJ29" s="6" t="s">
         <v>880</v>
       </c>
+      <c r="BL29" s="1" t="s">
+        <v>810</v>
+      </c>
       <c r="BR29" s="6" t="s">
         <v>742</v>
       </c>
@@ -13753,7 +13782,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="30" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>167</v>
       </c>
@@ -13918,7 +13947,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="31" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>52</v>
       </c>
@@ -14083,7 +14112,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="32" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>53</v>
       </c>
@@ -14245,7 +14274,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="33" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>168</v>
       </c>
@@ -14407,7 +14436,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="34" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>169</v>
       </c>
@@ -14566,7 +14595,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="35" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>170</v>
       </c>
@@ -14722,7 +14751,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="36" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>171</v>
       </c>
@@ -14857,7 +14886,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="37" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>54</v>
       </c>
@@ -14986,7 +15015,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="38" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>55</v>
       </c>
@@ -15115,7 +15144,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="39" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>56</v>
       </c>
@@ -15238,7 +15267,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="40" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>57</v>
       </c>
@@ -15352,7 +15381,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="41" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>58</v>
       </c>
@@ -15454,7 +15483,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="42" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>59</v>
       </c>
@@ -15513,6 +15542,9 @@
       <c r="AJ42" s="10" t="s">
         <v>864</v>
       </c>
+      <c r="AQ42" s="1" t="s">
+        <v>802</v>
+      </c>
       <c r="BG42" s="11" t="s">
         <v>881</v>
       </c>
@@ -15550,7 +15582,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="43" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>60</v>
       </c>
@@ -15606,6 +15638,9 @@
       <c r="AJ43" s="1" t="s">
         <v>867</v>
       </c>
+      <c r="AQ43" s="1" t="s">
+        <v>1014</v>
+      </c>
       <c r="BG43" s="11" t="s">
         <v>364</v>
       </c>
@@ -15643,7 +15678,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="44" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>61</v>
       </c>
@@ -15696,6 +15731,9 @@
       <c r="AJ44" s="1" t="s">
         <v>375</v>
       </c>
+      <c r="AQ44" s="1" t="s">
+        <v>1016</v>
+      </c>
       <c r="BG44" s="1" t="s">
         <v>956</v>
       </c>
@@ -15733,7 +15771,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="45" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>62</v>
       </c>
@@ -15786,6 +15824,9 @@
       <c r="AJ45" s="1" t="s">
         <v>868</v>
       </c>
+      <c r="AQ45" s="1" t="s">
+        <v>1015</v>
+      </c>
       <c r="BG45" s="1" t="s">
         <v>536</v>
       </c>
@@ -15823,7 +15864,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="46" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>63</v>
       </c>
@@ -15872,6 +15913,9 @@
       <c r="AJ46" s="1" t="s">
         <v>869</v>
       </c>
+      <c r="AQ46" s="1" t="s">
+        <v>740</v>
+      </c>
       <c r="BG46" s="1" t="s">
         <v>740</v>
       </c>
@@ -15906,7 +15950,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="47" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>172</v>
       </c>
@@ -15952,6 +15996,9 @@
       <c r="AJ47" s="1" t="s">
         <v>311</v>
       </c>
+      <c r="AQ47" s="1" t="s">
+        <v>741</v>
+      </c>
       <c r="BI47" s="1" t="s">
         <v>740</v>
       </c>
@@ -15977,7 +16024,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="48" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>64</v>
       </c>
@@ -16020,6 +16067,9 @@
       <c r="AJ48" s="1" t="s">
         <v>334</v>
       </c>
+      <c r="AQ48" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="CP48" s="1" t="s">
         <v>1024</v>
       </c>
@@ -16039,7 +16089,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="49" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>65</v>
       </c>
@@ -16082,6 +16132,9 @@
       <c r="AJ49" s="11" t="s">
         <v>954</v>
       </c>
+      <c r="AQ49" s="1" t="s">
+        <v>1043</v>
+      </c>
       <c r="CP49" s="1" t="s">
         <v>1025</v>
       </c>
@@ -16101,7 +16154,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="50" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>173</v>
       </c>
@@ -16144,6 +16197,9 @@
       <c r="AJ50" s="1" t="s">
         <v>955</v>
       </c>
+      <c r="AQ50" s="1" t="s">
+        <v>1044</v>
+      </c>
       <c r="CP50" s="1" t="s">
         <v>1026</v>
       </c>
@@ -16163,7 +16219,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="51" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>174</v>
       </c>
@@ -16206,6 +16262,9 @@
       <c r="AJ51" s="1" t="s">
         <v>959</v>
       </c>
+      <c r="AQ51" s="1" t="s">
+        <v>1045</v>
+      </c>
       <c r="CP51" s="1" t="s">
         <v>901</v>
       </c>
@@ -16222,7 +16281,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="52" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>175</v>
       </c>
@@ -16262,6 +16321,9 @@
       <c r="AI52" s="11" t="s">
         <v>954</v>
       </c>
+      <c r="AQ52" s="1" t="s">
+        <v>1046</v>
+      </c>
       <c r="CP52" s="1" t="s">
         <v>1027</v>
       </c>
@@ -16278,7 +16340,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="53" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>176</v>
       </c>
@@ -16328,7 +16390,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="54" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>177</v>
       </c>
@@ -16375,7 +16437,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="55" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>178</v>
       </c>
@@ -16425,7 +16487,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="56" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>66</v>
       </c>
@@ -16472,7 +16534,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="57" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>179</v>
       </c>
@@ -16516,7 +16578,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="58" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>67</v>
       </c>
@@ -16557,7 +16619,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="59" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>68</v>
       </c>
@@ -16598,7 +16660,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="60" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>69</v>
       </c>
@@ -16639,7 +16701,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="61" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>180</v>
       </c>
@@ -16677,7 +16739,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="62" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>253</v>
       </c>
@@ -16712,7 +16774,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="63" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>254</v>
       </c>
@@ -16744,7 +16806,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="64" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>181</v>
       </c>
@@ -16776,7 +16838,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="65" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>182</v>
       </c>
@@ -16805,7 +16867,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="66" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>70</v>
       </c>
@@ -16834,7 +16896,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="67" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>183</v>
       </c>
@@ -16860,7 +16922,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="68" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>255</v>
       </c>
@@ -16886,7 +16948,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="69" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>256</v>
       </c>
@@ -16912,7 +16974,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="70" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>257</v>
       </c>
@@ -16938,7 +17000,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="71" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>184</v>
       </c>
@@ -16964,7 +17026,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="72" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>185</v>
       </c>
@@ -16990,7 +17052,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="73" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>186</v>
       </c>
@@ -17016,7 +17078,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="74" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>71</v>
       </c>
@@ -17039,7 +17101,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="75" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>72</v>
       </c>
@@ -17062,7 +17124,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="76" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
         <v>258</v>
       </c>
@@ -17076,7 +17138,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="77" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>259</v>
       </c>
@@ -17090,7 +17152,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="78" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>260</v>
       </c>
@@ -17104,7 +17166,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="79" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>73</v>
       </c>
@@ -17112,7 +17174,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="80" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>74</v>
       </c>
@@ -17120,7 +17182,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="81" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>187</v>
       </c>
@@ -17128,7 +17190,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="82" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>188</v>
       </c>
@@ -17136,7 +17198,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="83" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>189</v>
       </c>
@@ -17144,7 +17206,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="84" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>75</v>
       </c>
@@ -17152,7 +17214,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="85" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>190</v>
       </c>
@@ -17160,7 +17222,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="86" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
         <v>76</v>
       </c>
@@ -17168,7 +17230,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="87" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>77</v>
       </c>
@@ -17176,7 +17238,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="88" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
         <v>78</v>
       </c>
@@ -17184,7 +17246,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="89" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
         <v>79</v>
       </c>
@@ -17192,7 +17254,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="90" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
         <v>80</v>
       </c>
@@ -17200,7 +17262,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="91" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>81</v>
       </c>
@@ -17208,7 +17270,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="92" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>82</v>
       </c>
@@ -17216,7 +17278,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="93" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
         <v>83</v>
       </c>
@@ -17224,7 +17286,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="94" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
         <v>84</v>
       </c>
@@ -17232,7 +17294,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="95" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
         <v>85</v>
       </c>
@@ -17240,7 +17302,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="96" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
         <v>86</v>
       </c>
@@ -17248,7 +17310,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="97" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
         <v>87</v>
       </c>
@@ -17256,7 +17318,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="98" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
         <v>88</v>
       </c>
@@ -17264,7 +17326,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="99" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
         <v>89</v>
       </c>
@@ -17272,7 +17334,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="100" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
         <v>90</v>
       </c>
@@ -17280,7 +17342,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="101" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
         <v>91</v>
       </c>
@@ -17288,7 +17350,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="102" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
         <v>92</v>
       </c>
@@ -17296,7 +17358,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="103" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
         <v>93</v>
       </c>
@@ -17304,7 +17366,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="104" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
         <v>94</v>
       </c>
@@ -17312,7 +17374,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="105" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
         <v>95</v>
       </c>
@@ -17320,7 +17382,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="106" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
         <v>96</v>
       </c>
@@ -17328,7 +17390,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="107" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
         <v>97</v>
       </c>
@@ -17336,7 +17398,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="108" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
         <v>98</v>
       </c>
@@ -17344,7 +17406,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="109" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
         <v>99</v>
       </c>
@@ -17352,7 +17414,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="110" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
         <v>100</v>
       </c>
@@ -17360,7 +17422,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="111" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
         <v>101</v>
       </c>
@@ -17368,7 +17430,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="112" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
         <v>102</v>
       </c>
@@ -17376,7 +17438,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="113" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
         <v>103</v>
       </c>
@@ -17384,7 +17446,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="114" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="s">
         <v>104</v>
       </c>
@@ -17392,7 +17454,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="115" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="s">
         <v>105</v>
       </c>
@@ -17400,7 +17462,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="116" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>106</v>
       </c>
@@ -17408,7 +17470,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="117" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>107</v>
       </c>
@@ -17416,7 +17478,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="118" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>108</v>
       </c>
@@ -17424,7 +17486,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="119" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>109</v>
       </c>
@@ -17432,7 +17494,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="120" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>110</v>
       </c>
@@ -17440,7 +17502,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="121" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>111</v>
       </c>
@@ -17448,7 +17510,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="122" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>112</v>
       </c>
@@ -17456,7 +17518,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="123" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>113</v>
       </c>
@@ -17464,7 +17526,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="124" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>114</v>
       </c>
@@ -17472,7 +17534,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="125" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>115</v>
       </c>
@@ -17480,7 +17542,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="126" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>116</v>
       </c>
@@ -17488,7 +17550,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="127" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>117</v>
       </c>
@@ -17496,7 +17558,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="128" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>118</v>
       </c>
@@ -17504,7 +17566,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="129" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>119</v>
       </c>
@@ -17512,7 +17574,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="130" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>120</v>
       </c>
@@ -17520,7 +17582,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="131" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>121</v>
       </c>
@@ -17528,7 +17590,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="132" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>122</v>
       </c>
@@ -17536,7 +17598,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="133" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>123</v>
       </c>
@@ -17544,7 +17606,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="134" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>191</v>
       </c>
@@ -17552,7 +17614,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="135" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>124</v>
       </c>
@@ -17560,7 +17622,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="136" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>125</v>
       </c>
@@ -17568,7 +17630,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="137" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>126</v>
       </c>
@@ -17576,7 +17638,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="138" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>127</v>
       </c>
@@ -17584,7 +17646,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="139" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>128</v>
       </c>
@@ -17592,7 +17654,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="140" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>129</v>
       </c>
@@ -17600,7 +17662,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="141" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>130</v>
       </c>
@@ -17608,7 +17670,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="142" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>131</v>
       </c>
@@ -17616,7 +17678,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="143" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>132</v>
       </c>
@@ -17624,7 +17686,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="144" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>133</v>
       </c>
@@ -17632,7 +17694,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="145" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>192</v>
       </c>
@@ -17640,7 +17702,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="146" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>134</v>
       </c>
@@ -17648,7 +17710,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="147" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>135</v>
       </c>
@@ -17656,7 +17718,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="148" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
         <v>136</v>
       </c>
@@ -17664,7 +17726,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="149" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
         <v>137</v>
       </c>
@@ -17672,7 +17734,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="150" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>138</v>
       </c>
@@ -17680,7 +17742,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="151" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
         <v>139</v>
       </c>
@@ -17688,12 +17750,12 @@
         <v>604</v>
       </c>
     </row>
-    <row r="152" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>837</v>
       </c>
     </row>
-    <row r="153" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
         <v>261</v>
       </c>
@@ -17701,7 +17763,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="154" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>193</v>
       </c>
@@ -17709,7 +17771,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="155" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
         <v>140</v>
       </c>
@@ -17717,7 +17779,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="156" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
         <v>141</v>
       </c>
@@ -17725,7 +17787,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="157" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
         <v>142</v>
       </c>
@@ -17733,7 +17795,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="158" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
         <v>143</v>
       </c>
@@ -17741,7 +17803,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="159" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
         <v>194</v>
       </c>
@@ -17749,7 +17811,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="160" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
         <v>144</v>
       </c>
@@ -17757,7 +17819,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="161" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
         <v>195</v>
       </c>
@@ -17765,7 +17827,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="162" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
         <v>196</v>
       </c>
@@ -17773,1452 +17835,1452 @@
         <v>613</v>
       </c>
     </row>
-    <row r="163" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="164" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="165" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="166" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="167" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="168" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="169" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="170" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="171" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="172" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="173" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="174" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A174" s="4" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="175" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A175" s="4" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="176" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A176" s="4" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A177" s="4" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A178" s="4" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A179" s="4" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180" s="4" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A181" s="4" t="s">
         <v>616</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A182" s="4" t="s">
         <v>615</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A183" s="5" t="s">
         <v>617</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A184" s="4" t="s">
         <v>618</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A185" s="4" t="s">
         <v>620</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186" s="4" t="s">
         <v>619</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A187" s="4" t="s">
         <v>621</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188" s="4" t="s">
         <v>622</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A189" s="4" t="s">
         <v>623</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A190" s="4" t="s">
         <v>625</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A191" s="4" t="s">
         <v>624</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192" s="4" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193" s="5" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A194" s="4" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195" s="4" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A196" s="4" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A197" s="4" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A198" s="4" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A199" s="4" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A200" s="4" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A201" s="4" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A202" s="4" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A203" s="4" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A204" s="4" t="s">
         <v>626</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A205" s="4" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A206" s="4" t="s">
         <v>630</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A207" s="4" t="s">
         <v>631</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A208" s="4" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A209" s="4" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A210" s="4" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A211" s="4" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A212" s="4" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A213" s="4" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A214" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A215" s="4" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A216" s="4" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A217" s="4" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A218" s="4" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A219" s="4" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A220" s="4" t="s">
         <v>633</v>
       </c>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A221" s="4" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A222" s="4" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A223" s="4" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A224" s="4" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A225" s="4" t="s">
         <v>636</v>
       </c>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A226" s="4" t="s">
         <v>637</v>
       </c>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A227" s="4" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A228" s="4" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A229" s="4" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A230" s="4" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A231" s="4" t="s">
         <v>638</v>
       </c>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A232" s="4" t="s">
         <v>639</v>
       </c>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A233" s="4" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A234" s="4" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A235" s="4" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A236" s="4" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A237" s="4" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A238" s="4" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A239" s="4" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A240" s="4" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A241" s="4" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A242" s="4" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A243" s="4" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A244" s="4" t="s">
         <v>642</v>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A245" s="4" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A246" s="4" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A247" s="4" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A248" s="4" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A249" s="4" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A250" s="4" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A251" s="4" t="s">
         <v>646</v>
       </c>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A252" s="4" t="s">
         <v>647</v>
       </c>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A253" s="4" t="s">
         <v>648</v>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A254" s="4" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A255" s="4" t="s">
         <v>650</v>
       </c>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A256" s="4" t="s">
         <v>649</v>
       </c>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A257" s="4" t="s">
         <v>551</v>
       </c>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A258" s="4" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A259" s="4" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A260" s="4" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A261" s="4" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A262" s="4" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A263" s="4" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A264" s="4" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A265" s="4" t="s">
         <v>652</v>
       </c>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A266" s="4" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A267" s="4" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A268" s="4" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A269" s="4" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A270" s="4" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A271" s="4" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A272" s="4" t="s">
         <v>655</v>
       </c>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A273" s="4" t="s">
         <v>656</v>
       </c>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A274" s="4" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A275" s="4" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A276" s="4" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A277" s="4" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A278" s="4" t="s">
         <v>657</v>
       </c>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A279" s="4" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A280" s="4" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A281" s="4" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A282" s="4" t="s">
         <v>662</v>
       </c>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A283" s="4" t="s">
         <v>660</v>
       </c>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A284" s="4" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A285" s="4" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A286" s="4" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A287" s="4" t="s">
         <v>574</v>
       </c>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A288" s="4" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A289" s="4" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A290" s="4" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A291" s="4" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A292" s="4" t="s">
         <v>663</v>
       </c>
     </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A293" s="4" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A294" s="4" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A295" s="4" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A296" s="4" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A297" s="4" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A298" s="4" t="s">
         <v>573</v>
       </c>
     </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A299" s="4" t="s">
         <v>664</v>
       </c>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A300" s="4" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A301" s="4" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A302" s="4" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A303" s="4" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A304" s="4" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A305" s="4" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A306" s="4" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A307" s="4" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A308" s="4" t="s">
         <v>669</v>
       </c>
     </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A309" s="4" t="s">
         <v>668</v>
       </c>
     </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A310" s="4" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A311" s="4" t="s">
         <v>667</v>
       </c>
     </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A312" s="4" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A313" s="4" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A314" s="4" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A315" s="4" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A316" s="4" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A317" s="4" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A318" s="4" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A319" s="4" t="s">
         <v>595</v>
       </c>
     </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A320" s="4" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A321" s="4" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A322" s="4" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A323" s="4" t="s">
         <v>674</v>
       </c>
     </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A324" s="4" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A325" s="4" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A326" s="4" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A327" s="4" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A328" s="4" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A329" s="4" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A330" s="4" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A331" s="4" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A332" s="4" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A333" s="4" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A334" s="4" t="s">
         <v>672</v>
       </c>
     </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A335" s="4" t="s">
         <v>670</v>
       </c>
     </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A336" s="4" t="s">
         <v>671</v>
       </c>
     </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A337" s="4" t="s">
         <v>678</v>
       </c>
     </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A338" s="4" t="s">
         <v>676</v>
       </c>
     </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A339" s="4" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A340" s="4" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A341" s="4" t="s">
         <v>677</v>
       </c>
     </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A342" s="4" t="s">
         <v>673</v>
       </c>
     </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A343" s="4" t="s">
         <v>675</v>
       </c>
     </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A344" s="4" t="s">
         <v>679</v>
       </c>
     </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A345" s="4" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A346" s="4" t="s">
         <v>680</v>
       </c>
     </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A347" s="4" t="s">
         <v>683</v>
       </c>
     </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A348" s="4" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A349" s="4" t="s">
         <v>682</v>
       </c>
     </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A350" s="4" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A351" s="4" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A352" s="4" t="s">
         <v>605</v>
       </c>
     </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A353" s="4" t="s">
         <v>684</v>
       </c>
     </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A354" s="4" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A355" s="4" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A356" s="4" t="s">
         <v>689</v>
       </c>
     </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A357" s="4" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A358" s="4" t="s">
         <v>691</v>
       </c>
     </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A359" s="4" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A360" s="4" t="s">
         <v>690</v>
       </c>
     </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A361" s="4" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A362" s="4" t="s">
         <v>692</v>
       </c>
     </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A363" s="4" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A364" s="4" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A365" s="4" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A366" s="4" t="s">
         <v>695</v>
       </c>
     </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A367" s="4" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A368" s="4" t="s">
         <v>696</v>
       </c>
     </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A369" s="4" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A370" s="4" t="s">
         <v>697</v>
       </c>
     </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A371" s="4" t="s">
         <v>698</v>
       </c>
     </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A372" s="4" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A373" s="4" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A374" s="4" t="s">
         <v>699</v>
       </c>
     </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A375" s="4" t="s">
         <v>701</v>
       </c>
     </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A376" s="4" t="s">
         <v>700</v>
       </c>
     </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A377" s="4" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A378" s="4" t="s">
         <v>702</v>
       </c>
     </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A379" s="4" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A380" s="4" t="s">
         <v>703</v>
       </c>
     </row>
-    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A381" s="4" t="s">
         <v>704</v>
       </c>
     </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A382" s="4" t="s">
         <v>706</v>
       </c>
     </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A383" s="4" t="s">
         <v>708</v>
       </c>
     </row>
-    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A384" s="4" t="s">
         <v>707</v>
       </c>
     </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A385" s="4" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A386" s="4" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A387" s="4" t="s">
         <v>711</v>
       </c>
     </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A388" s="4" t="s">
         <v>712</v>
       </c>
     </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A389" s="4" t="s">
         <v>713</v>
       </c>
     </row>
-    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A390" s="4" t="s">
         <v>710</v>
       </c>
     </row>
-    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A391" s="4" t="s">
         <v>715</v>
       </c>
     </row>
-    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A392" s="4" t="s">
         <v>716</v>
       </c>
     </row>
-    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A393" s="4" t="s">
         <v>714</v>
       </c>
     </row>
-    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A394" s="4" t="s">
         <v>717</v>
       </c>
     </row>
-    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A395" s="4" t="s">
         <v>720</v>
       </c>
     </row>
-    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A396" s="4" t="s">
         <v>719</v>
       </c>
     </row>
-    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A397" s="4" t="s">
         <v>721</v>
       </c>
     </row>
-    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A398" s="4" t="s">
         <v>718</v>
       </c>
     </row>
-    <row r="399" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A399" s="4" t="s">
         <v>722</v>
       </c>
     </row>
-    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A400" s="4" t="s">
         <v>723</v>
       </c>
     </row>
-    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A401" s="4" t="s">
         <v>724</v>
       </c>
     </row>
-    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A402" s="4" t="s">
         <v>725</v>
       </c>
     </row>
-    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A403" s="4" t="s">
         <v>726</v>
       </c>
     </row>
-    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A404" s="4" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A405" s="4" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A406" s="4" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A407" s="4" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A408" s="4" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A409" s="4" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A410" s="4" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A411" s="4" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A412" s="4" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A413" s="4" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A414" s="4" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A415" s="4" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A416" s="4" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A417" s="7" t="s">
         <v>731</v>
       </c>
     </row>
-    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A418" s="7" t="s">
         <v>728</v>
       </c>
     </row>
-    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A419" s="7" t="s">
         <v>732</v>
       </c>
     </row>
-    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A420" s="7" t="s">
         <v>730</v>
       </c>
     </row>
-    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A421" s="7" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A422" s="7" t="s">
         <v>734</v>
       </c>
     </row>
-    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A423" s="7" t="s">
         <v>733</v>
       </c>
     </row>
-    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A424" s="7" t="s">
         <v>747</v>
       </c>
     </row>
-    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A425" s="7" t="s">
         <v>838</v>
       </c>
     </row>
-    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A426" s="7" t="s">
         <v>839</v>
       </c>
     </row>
-    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A427" s="7" t="s">
         <v>840</v>
       </c>
     </row>
-    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A428" s="7" t="s">
         <v>805</v>
       </c>
     </row>
-    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A429" s="7" t="s">
         <v>841</v>
       </c>
     </row>
-    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A430" s="7" t="s">
         <v>842</v>
       </c>
     </row>
-    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A431" s="7" t="s">
         <v>843</v>
       </c>
     </row>
-    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A432" s="7" t="s">
         <v>844</v>
       </c>
     </row>
-    <row r="433" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A433" s="7" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="434" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A434" s="7" t="s">
         <v>829</v>
       </c>
     </row>
-    <row r="435" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A435" s="7" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A436" s="7" t="s">
         <v>845</v>
       </c>
     </row>
-    <row r="437" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A437" s="7" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="438" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A438" s="7" t="s">
         <v>846</v>
       </c>
     </row>
-    <row r="439" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A439" s="7" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A440" s="7" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A441" s="4" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A442" s="4" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A443" s="4" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A444" s="4" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A445" s="4" t="s">
         <v>745</v>
       </c>
     </row>
-    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A446" s="4" t="s">
         <v>847</v>
       </c>
     </row>
-    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A447" s="4" t="s">
         <v>848</v>
       </c>
     </row>
-    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A448" s="4" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A449" s="1" t="s">
         <v>783</v>
       </c>
     </row>
-    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A450" s="1" t="s">
         <v>784</v>
       </c>
     </row>
-    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A451" s="4" t="s">
         <v>806</v>
       </c>
     </row>
-    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A452" s="4" t="s">
         <v>807</v>
       </c>

</xml_diff>